<commit_message>
Database_Schema document file updated and added
</commit_message>
<xml_diff>
--- a/Documents/Social_Complaints_Database.xlsx
+++ b/Documents/Social_Complaints_Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
   <si>
     <t>government_officials_profile_tbl</t>
   </si>
@@ -270,9 +270,6 @@
     <t>complaint_category_name</t>
   </si>
   <si>
-    <t>government_department_id (fk)</t>
-  </si>
-  <si>
     <t>government_official_address_id  (pk)</t>
   </si>
   <si>
@@ -324,15 +321,9 @@
     <t>citizen_id  (fk)</t>
   </si>
   <si>
-    <t>vendor_id  (fk)</t>
-  </si>
-  <si>
     <t>worker_id  (fk)</t>
   </si>
   <si>
-    <t>government_official _id  (fk)</t>
-  </si>
-  <si>
     <t>PROJECT NAME</t>
   </si>
   <si>
@@ -349,13 +340,85 @@
   </si>
   <si>
     <t>admin_password</t>
+  </si>
+  <si>
+    <t>INT 
+AUTO_INCREMENT 
+PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>VARBINARY(200)</t>
+  </si>
+  <si>
+    <t>VARBINARY(200</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>VARCHAR(200)</t>
+  </si>
+  <si>
+    <t>VARCHAR(200) 
+NOT NULL 
+PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>INT 
+AUTO_INCREMENT 
+FOREIGN KEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR(200) 
+NOT NULL </t>
+  </si>
+  <si>
+    <t>workers_address_information_tbl</t>
+  </si>
+  <si>
+    <t>profile_image</t>
+  </si>
+  <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>INT 
+FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>complaint_subcategory_id  (fk)</t>
+  </si>
+  <si>
+    <t>VARCHAR(255) 
+PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>VARBINARY</t>
+  </si>
+  <si>
+    <t>citizen_address_id  (fk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR(200) </t>
+  </si>
+  <si>
+    <t>workers_address_id  (fk)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,31 +451,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
@@ -427,19 +469,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -450,13 +479,20 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,8 +515,14 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -581,40 +623,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,446 +987,769 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" style="4" customWidth="1"/>
+    <col min="2" max="4" width="44.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="51.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="13" t="s">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="D8" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="8" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="G12" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="I12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="C17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M29" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="D32" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="13"/>
+    </row>
+    <row r="35" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-    </row>
-    <row r="22" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-    </row>
-    <row r="30" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-    </row>
-    <row r="32" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+      <c r="B44" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="C44" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="45" spans="1:11" ht="48" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>